<commit_message>
Färger i protokoll för armbindlar
</commit_message>
<xml_diff>
--- a/mallar/import/Sm2019/extraktion-v3-sm2019.xlsx
+++ b/mallar/import/Sm2019/extraktion-v3-sm2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\import\Sm2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4EF111-481F-41E2-B231-22EBF9B6522F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FCF13E-35B5-4105-A58C-65F1D293B741}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="5" xr2:uid="{EF1B5C3D-AC33-4B29-A729-47C982E6613A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{EF1B5C3D-AC33-4B29-A729-47C982E6613A}"/>
   </bookViews>
   <sheets>
     <sheet name="ekipage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="246">
   <si>
     <t>Christina Müller</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>Vit 16</t>
+  </si>
+  <si>
+    <t>Frillesås juniorlag</t>
   </si>
 </sst>
 </file>
@@ -1141,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89E699B4-799D-435C-8FEE-CA3AE7CBAE4C}">
   <dimension ref="A1:W65"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1442,6 +1445,9 @@
       <c r="V4" t="s">
         <v>90</v>
       </c>
+      <c r="W4" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A5">
@@ -4469,7 +4475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F6038BD-E98A-4EC9-82EE-E489CA9E309A}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>

</xml_diff>